<commit_message>
add script for resyncing data
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_client_tracing.xlsx
+++ b/config/default/forms/app/hts_client_tracing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -249,7 +249,7 @@
     <t xml:space="preserve">_1779_phoneWhyNot_99DCT</t>
   </si>
   <si>
-    <t xml:space="preserve">Why was phone contact not attempted?</t>
+    <t xml:space="preserve">Why was phone tracing not successful?</t>
   </si>
   <si>
     <t xml:space="preserve">${_159811_outcome_99DCT}=”_1118_notReached_99DCT” and ${_164966_tracingType_99DCT}=”_1650_phone_99DCT”</t>
@@ -261,7 +261,7 @@
     <t xml:space="preserve">_5622_phoneSpecify_99DCT</t>
   </si>
   <si>
-    <t xml:space="preserve">Specify why  phone contact not attempted?</t>
+    <t xml:space="preserve">Other(specify)?</t>
   </si>
   <si>
     <t xml:space="preserve">no</t>
@@ -276,7 +276,7 @@
     <t xml:space="preserve">_1779_physicalWhyNot_99DCT</t>
   </si>
   <si>
-    <t xml:space="preserve">Why was physical contacting not attempted?</t>
+    <t xml:space="preserve">Why was physical tracing not successful?</t>
   </si>
   <si>
     <t xml:space="preserve">${_159811_outcome_99DCT}=”_1118_notReached_99DCT” and ${_164966_tracingType_99DCT}=”_164965_physical_99DCT”</t>
@@ -285,7 +285,7 @@
     <t xml:space="preserve">_5622_physicalSpecify_99DCT</t>
   </si>
   <si>
-    <t xml:space="preserve">Specify why physical contacting not attempted?</t>
+    <t xml:space="preserve">Other (specify)?</t>
   </si>
   <si>
     <t xml:space="preserve">${_1779_physicalWhyNot_99DCT}=”_5622_otherInfo_99DCT”</t>
@@ -646,7 +646,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="DD\-MM\-YYYY\ HH\-MM\-SS"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -735,12 +735,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
@@ -821,7 +815,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -886,10 +880,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -898,7 +888,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -930,7 +920,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -938,7 +928,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -951,232 +941,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -1496,25 +1261,25 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="72.265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2397959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.4285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="40.3163265306123"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="91.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.3673469387755"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="36.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.7295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.015306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.9081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.1377551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.6683673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="94.4030612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.9081632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.9081632653061"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="37.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="17.9081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,7 +2261,7 @@
         <v>68</v>
       </c>
       <c r="D29" s="12"/>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="13" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="11"/>
@@ -2584,7 +2349,7 @@
       <c r="X31" s="8"/>
       <c r="Y31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
         <v>77</v>
       </c>
@@ -2712,7 +2477,7 @@
       <c r="X35" s="8"/>
       <c r="Y35" s="8"/>
     </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
         <v>77</v>
       </c>
@@ -2977,7 +2742,7 @@
       <c r="B45" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="16" t="s">
         <v>100</v>
       </c>
       <c r="D45" s="8"/>
@@ -3012,7 +2777,7 @@
       <c r="B46" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="16" t="s">
         <v>103</v>
       </c>
       <c r="D46" s="8"/>
@@ -3077,7 +2842,7 @@
       <c r="A48" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
         <v>107</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -3113,7 +2878,7 @@
       <c r="B49" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="18" t="s">
         <v>110</v>
       </c>
       <c r="D49" s="4"/>
@@ -3150,7 +2915,7 @@
       <c r="B50" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="18" t="s">
         <v>114</v>
       </c>
       <c r="D50" s="4"/>
@@ -3183,7 +2948,7 @@
     <row r="51" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
-      <c r="C51" s="19"/>
+      <c r="C51" s="18"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
@@ -3244,10 +3009,10 @@
       <c r="A53" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="19" t="s">
         <v>119</v>
       </c>
       <c r="D53" s="8"/>
@@ -3281,10 +3046,10 @@
       <c r="A54" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="19" t="s">
         <v>122</v>
       </c>
       <c r="D54" s="8"/>
@@ -3318,10 +3083,10 @@
       <c r="A55" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="19" t="s">
         <v>125</v>
       </c>
       <c r="D55" s="8"/>
@@ -3390,10 +3155,10 @@
       <c r="A57" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="19" t="s">
         <v>130</v>
       </c>
       <c r="D57" s="4"/>
@@ -3427,10 +3192,10 @@
       <c r="A58" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C58" s="19" t="s">
         <v>133</v>
       </c>
       <c r="D58" s="4"/>
@@ -3464,10 +3229,10 @@
       <c r="A59" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" s="19" t="s">
         <v>136</v>
       </c>
       <c r="D59" s="4"/>
@@ -3501,10 +3266,10 @@
       <c r="A60" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C60" s="20" t="s">
+      <c r="C60" s="19" t="s">
         <v>139</v>
       </c>
       <c r="D60" s="4"/>
@@ -3538,10 +3303,10 @@
       <c r="A61" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="19" t="s">
         <v>142</v>
       </c>
       <c r="D61" s="4"/>
@@ -3573,8 +3338,8 @@
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="20"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="19"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -3637,10 +3402,10 @@
       <c r="A64" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B64" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="19" t="s">
         <v>147</v>
       </c>
       <c r="D64" s="4"/>
@@ -3674,10 +3439,10 @@
       <c r="A65" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="19" t="s">
         <v>133</v>
       </c>
       <c r="D65" s="4"/>
@@ -3711,10 +3476,10 @@
       <c r="A66" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="19" t="s">
         <v>151</v>
       </c>
       <c r="D66" s="4"/>
@@ -3748,10 +3513,10 @@
       <c r="A67" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="19" t="s">
         <v>154</v>
       </c>
       <c r="D67" s="4"/>
@@ -3785,10 +3550,10 @@
       <c r="A68" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="19" t="s">
         <v>139</v>
       </c>
       <c r="D68" s="4"/>
@@ -3822,10 +3587,10 @@
       <c r="A69" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="19" t="s">
         <v>142</v>
       </c>
       <c r="D69" s="4"/>
@@ -3854,76 +3619,76 @@
       <c r="Y69" s="4"/>
     </row>
     <row r="70" s="12" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="21" t="s">
+      <c r="A70" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B70" s="21" t="s">
+      <c r="B70" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="C70" s="22" t="s">
+      <c r="C70" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="D70" s="21"/>
-      <c r="E70" s="23" t="s">
+      <c r="D70" s="20"/>
+      <c r="E70" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="F70" s="21" t="s">
+      <c r="F70" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="G70" s="21"/>
-      <c r="H70" s="21"/>
-      <c r="I70" s="21"/>
-      <c r="J70" s="21"/>
-      <c r="K70" s="21"/>
-      <c r="L70" s="21"/>
-      <c r="M70" s="21"/>
-      <c r="N70" s="21"/>
-      <c r="O70" s="21"/>
-      <c r="P70" s="21"/>
-      <c r="Q70" s="21"/>
-      <c r="R70" s="21"/>
-      <c r="S70" s="21"/>
-      <c r="T70" s="21"/>
-      <c r="U70" s="21"/>
-      <c r="V70" s="21"/>
-      <c r="W70" s="21"/>
-      <c r="X70" s="21"/>
-      <c r="Y70" s="21"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="20"/>
+      <c r="M70" s="20"/>
+      <c r="N70" s="20"/>
+      <c r="O70" s="20"/>
+      <c r="P70" s="20"/>
+      <c r="Q70" s="20"/>
+      <c r="R70" s="20"/>
+      <c r="S70" s="20"/>
+      <c r="T70" s="20"/>
+      <c r="U70" s="20"/>
+      <c r="V70" s="20"/>
+      <c r="W70" s="20"/>
+      <c r="X70" s="20"/>
+      <c r="Y70" s="20"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="24" t="s">
+      <c r="A71" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B71" s="24" t="s">
+      <c r="B71" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C71" s="23" t="s">
         <v>163</v>
       </c>
       <c r="D71" s="5"/>
-      <c r="E71" s="25" t="s">
+      <c r="E71" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="24"/>
-      <c r="J71" s="24"/>
-      <c r="K71" s="24"/>
-      <c r="L71" s="24"/>
-      <c r="M71" s="24"/>
-      <c r="N71" s="24"/>
-      <c r="O71" s="24"/>
-      <c r="P71" s="24"/>
-      <c r="Q71" s="24"/>
-      <c r="R71" s="24"/>
-      <c r="S71" s="24"/>
-      <c r="T71" s="24"/>
-      <c r="U71" s="24"/>
-      <c r="V71" s="24"/>
-      <c r="W71" s="24"/>
-      <c r="X71" s="24"/>
-      <c r="Y71" s="24"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
+      <c r="H71" s="23"/>
+      <c r="I71" s="23"/>
+      <c r="J71" s="23"/>
+      <c r="K71" s="23"/>
+      <c r="L71" s="23"/>
+      <c r="M71" s="23"/>
+      <c r="N71" s="23"/>
+      <c r="O71" s="23"/>
+      <c r="P71" s="23"/>
+      <c r="Q71" s="23"/>
+      <c r="R71" s="23"/>
+      <c r="S71" s="23"/>
+      <c r="T71" s="23"/>
+      <c r="U71" s="23"/>
+      <c r="V71" s="23"/>
+      <c r="W71" s="23"/>
+      <c r="X71" s="23"/>
+      <c r="Y71" s="23"/>
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
@@ -4000,487 +3765,462 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" priority="10" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="10" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"choice_filter"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="notContainsText" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="2"/>
+    <cfRule type="notContainsText" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"default"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Y1">
-    <cfRule type="cellIs" priority="13" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="13" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I30:I31,I27">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>AND($I27 = "", $A27 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31,C27">
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>AND(AND(NOT($A27 = "end group"), NOT($A27 = "end repeat"), NOT($A27 = "")), $C27 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B31,B27">
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>AND(AND(NOT($A27 = "end group"), NOT($A27 = "end repeat"), NOT($A27 = "")), $B27 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H30:H31,H27">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND(NOT($G27 = ""), $H27 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A30,A27">
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+  <conditionalFormatting sqref="A30">
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
-    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+  <conditionalFormatting sqref="I32:I34">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($I32 = "", $A32 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:C34">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND(AND(NOT($A32 = "end group"), NOT($A32 = "end repeat"), NOT($A32 = "")), $C32 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:B34">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND(AND(NOT($A32 = "end group"), NOT($A32 = "end repeat"), NOT($A32 = "")), $B32 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:A34">
+    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32:I34">
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($I32 = "", $A32 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32:C34">
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND(AND(NOT($A32 = "end group"), NOT($A32 = "end repeat"), NOT($A32 = "")), $C32 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32:B34">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND(AND(NOT($A32 = "end group"), NOT($A32 = "end repeat"), NOT($A32 = "")), $B32 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32:A34">
-    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+  <conditionalFormatting sqref="H32:H34">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND(NOT($G32 = ""), $H32 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="containsText" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A31="begin group", NOT($B31 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A31="end group", $B31 = "", $C31 = "", $D31 = "", $E31 = "", $F31 = "", $G31 = "", $H31 = "", $I31 = "", $J31 = "", $K31 = "", $L31 = "", $M31 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A31="begin repeat", NOT($B31 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A31="end repeat", $B31 = "", $C31 = "", $D31 = "", $E31 = "", $F31 = "", $G31 = "", $H31 = "", $I31 = "", $J31 = "", $K31 = "", $L31 = "", $M31 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($I38 = "", $A38 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
+    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $C38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $B38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32:H34">
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND(NOT($G32 = ""), $H32 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($A31="begin group", NOT($B31 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($A31="end group", $B31 = "", $C31 = "", $D31 = "", $E31 = "", $F31 = "", $G31 = "", $H31 = "", $I31 = "", $J31 = "", $K31 = "", $L31 = "", $M31 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+  <conditionalFormatting sqref="H38">
+    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND(NOT($G38 = ""), $H38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23:Y25">
+    <cfRule type="containsText" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23:Y25">
+    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($A31="begin repeat", NOT($B31 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($A31="end repeat", $B31 = "", $C31 = "", $D31 = "", $E31 = "", $F31 = "", $G31 = "", $H31 = "", $I31 = "", $J31 = "", $K31 = "", $L31 = "", $M31 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($I38 = "", $A38 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
-    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $C38 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
-    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
-      <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $B38 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
-    <cfRule type="cellIs" priority="35" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+  <conditionalFormatting sqref="A23:A25">
+    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>AND(NOT($G38 = ""), $H38 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23:Y25">
-    <cfRule type="containsText" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23:Y25">
-    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+  <conditionalFormatting sqref="A72">
+    <cfRule type="containsText" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+      <formula>AND($A72="begin group", NOT($B72 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
+    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A72="end group", $B72 = "", $C72 = "", $D72 = "", $E72 = "", $F72 = "", $G72 = "", $H72 = "", $I72 = "", $J72 = "", $K72 = "", $L72 = "", $M72 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
+    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A25">
-    <cfRule type="cellIs" priority="39" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+  <conditionalFormatting sqref="A72">
+    <cfRule type="cellIs" priority="39" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="containsText" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="13"/>
+    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A72="begin repeat", NOT($B72 = ""))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
-      <formula>AND($A72="begin group", NOT($B72 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
-    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>AND($A72="end group", $B72 = "", $C72 = "", $D72 = "", $E72 = "", $F72 = "", $G72 = "", $H72 = "", $I72 = "", $J72 = "", $K72 = "", $L72 = "", $M72 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
-    <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A72="end repeat", $B72 = "", $C72 = "", $D72 = "", $E72 = "", $F72 = "", $G72 = "", $H72 = "", $I72 = "", $J72 = "", $K72 = "", $L72 = "", $M72 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I35">
+    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($I35 = "", $A35 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $C35 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $B35 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="cellIs" priority="45" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(NOT($G35 = ""), $H35 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
+    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($I36 = "", $A36 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $C36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36">
+    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $B36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(NOT($G36 = ""), $H36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="containsText" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>AND($A36="begin group", NOT($B36 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+      <formula>AND($A36="end group", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="cellIs" priority="55" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
-    <cfRule type="cellIs" priority="44" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+  <conditionalFormatting sqref="E36">
+    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+      <formula>AND($A36="begin repeat", NOT($B36 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+      <formula>AND($A36="end repeat", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="containsText" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>AND($A35="begin group", NOT($B35 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>AND($A35="end group", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $G35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="cellIs" priority="61" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>AND($A35="begin repeat", NOT($B35 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>AND($A35="end repeat", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $G35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="containsText" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>AND($A52="begin group", NOT($B52 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A52="end group", $B52 = "", $C52 = "", $D52 = "", $E52 = "", $F52 = "", $G52 = "", $H52 = "", $I52 = "", $J52 = "", $K52 = "", $L52 = "", $M52 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A52="begin repeat", NOT($B52 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A52="end repeat", $B52 = "", $C52 = "", $D52 = "", $E52 = "", $F52 = "", $G52 = "", $H52 = "", $I52 = "", $J52 = "", $K52 = "", $L52 = "", $M52 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="cellIs" priority="70" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
-    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
-      <formula>AND($A72="begin repeat", NOT($B72 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A72">
-    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
-      <formula>AND($A72="end repeat", $B72 = "", $C72 = "", $D72 = "", $E72 = "", $F72 = "", $G72 = "", $H72 = "", $I72 = "", $J72 = "", $K72 = "", $L72 = "", $M72 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
-    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
-      <formula>AND($I35 = "", $A35 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
-      <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $C35 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
-    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
-      <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $B35 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
-    <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+  <conditionalFormatting sqref="A54:Y54">
+    <cfRule type="containsText" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:Y54">
+    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A54="begin group", NOT($B54 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:Y54">
+    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A54="end group", $B54 = "", $C54 = "", $D54 = "", $E54 = "", $F54 = "", $G54 = "", $H54 = "", $I54 = "", $J54 = "", $K54 = "", $L54 = "", $M54 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:Y54">
+    <cfRule type="cellIs" priority="74" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I54">
+    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+      <formula>AND($I54 = "", $A54 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+      <formula>AND(AND(NOT($A54 = "end group"), NOT($A54 = "end repeat"), NOT($A54 = "")), $C54 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
+    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+      <formula>AND(AND(NOT($A54 = "end group"), NOT($A54 = "end repeat"), NOT($A54 = "")), $B54 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="cellIs" priority="78" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
-      <formula>AND(NOT($G35 = ""), $H35 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
-      <formula>AND($I36 = "", $A36 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
-      <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $C36 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
-      <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $B36 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" priority="55" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+  <conditionalFormatting sqref="H54">
+    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+      <formula>AND(NOT($G54 = ""), $H54 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:Y54">
+    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+      <formula>AND($A54="begin repeat", NOT($B54 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:Y54">
+    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+      <formula>AND($A54="end repeat", $B54 = "", $C54 = "", $D54 = "", $E54 = "", $F54 = "", $G54 = "", $H54 = "", $I54 = "", $J54 = "", $K54 = "", $L54 = "", $M54 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55:Y55">
+    <cfRule type="containsText" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55:Y55">
+    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+      <formula>AND($A55="begin group", NOT($B55 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55:Y55">
+    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+      <formula>AND($A55="end group", $B55 = "", $C55 = "", $D55 = "", $E55 = "", $F55 = "", $G55 = "", $H55 = "", $I55 = "", $J55 = "", $K55 = "", $L55 = "", $M55 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55:Y55">
+    <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I55">
+    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+      <formula>AND($I55 = "", $A55 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+      <formula>AND(AND(NOT($A55 = "end group"), NOT($A55 = "end repeat"), NOT($A55 = "")), $C55 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B55">
+    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+      <formula>AND(AND(NOT($A55 = "end group"), NOT($A55 = "end repeat"), NOT($A55 = "")), $B55 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="cellIs" priority="89" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(NOT($G36 = ""), $H36 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="29"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
-      <formula>AND($A36="begin group", NOT($B36 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
-      <formula>AND($A36="end group", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" priority="60" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
+  <conditionalFormatting sqref="H55">
+    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+      <formula>AND(NOT($G55 = ""), $H55 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55:Y55">
+    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+      <formula>AND($A55="begin repeat", NOT($B55 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55:Y55">
+    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+      <formula>AND($A55="end repeat", $B55 = "", $C55 = "", $D55 = "", $E55 = "", $F55 = "", $G55 = "", $H55 = "", $I55 = "", $J55 = "", $K55 = "", $L55 = "", $M55 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$984, "begin group") = COUNTIF($A$1:$A$984, "end group"))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$975, "begin group") = COUNTIF($A$1:$A$984, "end group")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($I37 = "", $A37 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $C37 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $B37 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="cellIs" priority="98" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37">
+    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND(NOT($G37 = ""), $H37 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="containsText" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A37="begin group", NOT($B37 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A37="end group", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
-      <formula>AND($A36="begin repeat", NOT($B36 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
-      <formula>AND($A36="end repeat", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="35"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
-      <formula>AND($A35="begin group", NOT($B35 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
-      <formula>AND($A35="end group", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $G35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" priority="66" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>AND($A35="begin repeat", NOT($B35 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>AND($A35="end repeat", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $G35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="containsText" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="38"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>AND($A52="begin group", NOT($B52 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>AND($A52="end group", $B52 = "", $C52 = "", $D52 = "", $E52 = "", $F52 = "", $G52 = "", $H52 = "", $I52 = "", $J52 = "", $K52 = "", $L52 = "", $M52 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" priority="72" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>AND($A52="begin repeat", NOT($B52 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="expression" priority="74" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>AND($A52="end repeat", $B52 = "", $C52 = "", $D52 = "", $E52 = "", $F52 = "", $G52 = "", $H52 = "", $I52 = "", $J52 = "", $K52 = "", $L52 = "", $M52 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" priority="75" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="containsText" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="39"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>AND($A54="begin group", NOT($B54 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="78" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>AND($A54="end group", $B54 = "", $C54 = "", $D54 = "", $E54 = "", $F54 = "", $G54 = "", $H54 = "", $I54 = "", $J54 = "", $K54 = "", $L54 = "", $M54 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="cellIs" priority="79" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I54">
-    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
-      <formula>AND($I54 = "", $A54 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>AND(AND(NOT($A54 = "end group"), NOT($A54 = "end repeat"), NOT($A54 = "")), $C54 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
-    <cfRule type="expression" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>AND(AND(NOT($A54 = "end group"), NOT($A54 = "end repeat"), NOT($A54 = "")), $B54 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
-    <cfRule type="cellIs" priority="83" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H54">
-    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>AND(NOT($G54 = ""), $H54 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="85" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>AND($A54="begin repeat", NOT($B54 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>AND($A54="end repeat", $B54 = "", $C54 = "", $D54 = "", $E54 = "", $F54 = "", $G54 = "", $H54 = "", $I54 = "", $J54 = "", $K54 = "", $L54 = "", $M54 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="containsText" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="42"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
-      <formula>AND($A55="begin group", NOT($B55 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="expression" priority="89" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
-      <formula>AND($A55="end group", $B55 = "", $C55 = "", $D55 = "", $E55 = "", $F55 = "", $G55 = "", $H55 = "", $I55 = "", $J55 = "", $K55 = "", $L55 = "", $M55 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="cellIs" priority="90" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I55">
-    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
-      <formula>AND($I55 = "", $A55 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
-    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
-      <formula>AND(AND(NOT($A55 = "end group"), NOT($A55 = "end repeat"), NOT($A55 = "")), $C55 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B55">
-    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
-      <formula>AND(AND(NOT($A55 = "end group"), NOT($A55 = "end repeat"), NOT($A55 = "")), $B55 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="cellIs" priority="94" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H55">
-    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
-      <formula>AND(NOT($G55 = ""), $H55 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
-      <formula>AND($A55="begin repeat", NOT($B55 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>AND($A55="end repeat", $B55 = "", $C55 = "", $D55 = "", $E55 = "", $F55 = "", $G55 = "", $H55 = "", $I55 = "", $J55 = "", $K55 = "", $L55 = "", $M55 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$984, "begin group") = COUNTIF($A$1:$A$984, "end group"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$975, "begin group") = COUNTIF($A$1:$A$984, "end group")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="expression" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>AND($I37 = "", $A37 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $C37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
-    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $B37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>AND(NOT($G37 = ""), $H37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="15"/>
+    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>AND($A37="begin repeat", NOT($B37 = ""))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>AND($A37="begin group", NOT($B37 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>AND($A37="end group", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" priority="108" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
-      <formula>AND($A37="begin repeat", NOT($B37 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A37="end repeat", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4518,126 +4258,126 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.984693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.9642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.9081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4645,10 +4385,10 @@
       <c r="A13" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4656,10 +4396,10 @@
       <c r="A14" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4667,25 +4407,25 @@
       <c r="A15" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4693,10 +4433,10 @@
       <c r="A18" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4704,10 +4444,10 @@
       <c r="A19" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4715,10 +4455,10 @@
       <c r="A20" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>154</v>
       </c>
     </row>
@@ -4726,10 +4466,10 @@
       <c r="A21" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4737,10 +4477,10 @@
       <c r="A22" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="19" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4772,50 +4512,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.5663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.3673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.9081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="C2" s="29" t="n">
+      <c r="C2" s="28" t="n">
         <f aca="true">NOW()</f>
-        <v>44339.693595784</v>
-      </c>
-      <c r="D2" s="19" t="s">
+        <v>44347.4972521824</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="F2" s="19"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Re-test date allows date earlier than the initial test validation
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_client_tracing.xlsx
+++ b/config/default/forms/app/hts_client_tracing.xlsx
@@ -1,19 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Desktop\hts090621\app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B02029C-D6EB-415D-AB19-22202888AAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" tabRatio="996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="choices" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -24,629 +39,627 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="204">
   <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relevant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">appearance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constraint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constraint_message::en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">media::image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">begin group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./source = 'user'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">field-list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hidden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db:universal_client</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the patient's name?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db-object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kemr_uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMR Client Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient_telephone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO_LABEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/source_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">place_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/contact/_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">place_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/contact/name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../inputs/contact/contact/name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'15ed03d2-c972-11e9-a32f-2a2ae2dbcce4'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">encounter_type_uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">'9c0a7a57-62ff-4f75-babe-5835b0e921b7'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">encounter_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of trace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">. &lt; today()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Encounter date cannot be in the future</t>
-  </si>
-  <si>
-    <t xml:space="preserve">observation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracing Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one tracing_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_164966_tracingType_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracing Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">call_button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[&lt;span style='background-color:#F0F4FD; border:1px solid #007AC0; padding: 0.5em; border-radius: 4px; text-decoration:none; display: block; margin-left: auto; margin-right: auto; width: 40%; text-align: center;'&gt;&lt;i class="fa fa-phone" aria-hidden="true"&gt;&lt;/i&gt;&amp;nbsp;Call ${name}&lt;/span&gt;](tel://${phone})</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${_164966_tracingType_99DCT}='_1650_phone_99DCT' and ${patient_telephone}!=''</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_phone</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>relevant</t>
+  </si>
+  <si>
+    <t>appearance</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>constraint_message::en</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>choice_filter</t>
+  </si>
+  <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>media::image</t>
+  </si>
+  <si>
+    <t>begin group</t>
+  </si>
+  <si>
+    <t>inputs</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>./source = 'user'</t>
+  </si>
+  <si>
+    <t>field-list</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>Source ID</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>db:universal_client</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>What is the patient's name?</t>
+  </si>
+  <si>
+    <t>db-object</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>kemr_uuid</t>
+  </si>
+  <si>
+    <t>EMR Client Reference</t>
+  </si>
+  <si>
+    <t>patient_telephone</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>end group</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>NO_LABEL</t>
+  </si>
+  <si>
+    <t>../inputs/source</t>
+  </si>
+  <si>
+    <t>../inputs/source_id</t>
+  </si>
+  <si>
+    <t>place_id</t>
+  </si>
+  <si>
+    <t>../inputs/contact/_id</t>
+  </si>
+  <si>
+    <t>place_name</t>
+  </si>
+  <si>
+    <t>../inputs/contact/name</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>../inputs/contact/contact/name</t>
+  </si>
+  <si>
+    <t>form_uuid</t>
+  </si>
+  <si>
+    <t>'15ed03d2-c972-11e9-a32f-2a2ae2dbcce4'</t>
+  </si>
+  <si>
+    <t>encounter_type_uuid</t>
+  </si>
+  <si>
+    <t>'9c0a7a57-62ff-4f75-babe-5835b0e921b7'</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>encounter_date</t>
+  </si>
+  <si>
+    <t>Date of trace</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>. &lt; today()</t>
+  </si>
+  <si>
+    <t>Encounter date cannot be in the future</t>
+  </si>
+  <si>
+    <t>observation</t>
+  </si>
+  <si>
+    <t>Tracing Information</t>
+  </si>
+  <si>
+    <t>select_one tracing_type</t>
+  </si>
+  <si>
+    <t>_164966_tracingType_99DCT</t>
+  </si>
+  <si>
+    <t>Tracing Type</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>call_button</t>
+  </si>
+  <si>
+    <t>[&lt;span style='background-color:#F0F4FD; border:1px solid #007AC0; padding: 0.5em; border-radius: 4px; text-decoration:none; display: block; margin-left: auto; margin-right: auto; width: 40%; text-align: center;'&gt;&lt;i class="fa fa-phone" aria-hidden="true"&gt;&lt;/i&gt;&amp;nbsp;Call ${name}&lt;/span&gt;](tel://${phone})</t>
+  </si>
+  <si>
+    <t>${_164966_tracingType_99DCT}='_1650_phone_99DCT' and ${patient_telephone}!=''</t>
+  </si>
+  <si>
+    <t>no_phone</t>
   </si>
   <si>
     <t xml:space="preserve"> &lt;span style="color:red;font-weight:bold"&gt;${name} does not have a registered phone number&lt;/span&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">${_164966_tracingType_99DCT}='_1650_phone_99DCT' and ${patient_telephone}=''</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one contact_status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_159811_outcome_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracing Outcome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one reasons_phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1779_phoneWhyNot_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Why was phone tracing not successful?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${_159811_outcome_99DCT}=”_1118_notReached_99DCT” and ${_164966_tracingType_99DCT}=”_1650_phone_99DCT”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_5622_phoneSpecify_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other(specify)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
+    <t>${_164966_tracingType_99DCT}='_1650_phone_99DCT' and ${patient_telephone}=''</t>
+  </si>
+  <si>
+    <t>select_one contact_status</t>
+  </si>
+  <si>
+    <t>_159811_outcome_99DCT</t>
+  </si>
+  <si>
+    <t>Tracing Outcome</t>
+  </si>
+  <si>
+    <t>select_one reasons_phone</t>
+  </si>
+  <si>
+    <t>_1779_phoneWhyNot_99DCT</t>
+  </si>
+  <si>
+    <t>Why was phone tracing not successful?</t>
+  </si>
+  <si>
+    <t>${_159811_outcome_99DCT}=”_1118_notReached_99DCT” and ${_164966_tracingType_99DCT}=”_1650_phone_99DCT”</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>_5622_phoneSpecify_99DCT</t>
+  </si>
+  <si>
+    <t>Other(specify)?</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t xml:space="preserve">${_1779_phoneWhyNot_99DCT}=”_5622_other_99DCT” </t>
   </si>
   <si>
-    <t xml:space="preserve">select_one reasons_physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1779_physicalWhyNot_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Why was physical tracing not successful?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${_159811_outcome_99DCT}=”_1118_notReached_99DCT” and ${_164966_tracingType_99DCT}=”_164965_physical_99DCT”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_5622_physicalSpecify_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other (specify)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${_1779_physicalWhyNot_99DCT}=”_5622_otherInfo_99DCT”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linkage_alert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;span style="color:red;font-weight:bold"&gt;Please fill UPN in the linkage form once you submit this form&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${_159811_outcome_99DCT}='_1065_contactedAndLinked_99DCT'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_5622_remarks_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group_review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summary page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">field-list summary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n_submit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_Be sure you submit to complete this action._</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n_household_details_title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client details&lt;I class="fa fa-user"&gt;&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h1 yellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n_household_details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h4 style="text-align:center;"&gt;${place_name} ${head}&lt;/h4&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n_assessment_findings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assessment findings&lt;I class="fa fa-user"&gt;&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h1 blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**_Contact type_**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Physical tracing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_164966_tracingType_99DCT, '_1650_phone_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">li</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone tracing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_164966_tracingType_99DCT, '_164965_physical_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n_test_1_results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**_Status_**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contactedAndLinked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contacted and linked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_159811_outcome_99DCT, '_1065_contactedAndLinked_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cintactedNotLinked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contacted not linked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_159811_outcome_99DCT, '_1066_contactedNotLinked_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">voluntaryExit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not contacted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_159811_outcome_99DCT, '_1118_notReached_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n_hts_strategy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**_Reason not contacted (Phone)_**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locationNotAvailable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No locator information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_phoneWhyNot_99DCT, '_165073_locationMissing_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wrongLocation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incorrect locator information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_phoneWhyNot_99DCT, '_165072_incorrect_location_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">callsNotGoingThrough</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calls not going through</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_phoneWhyNot_99DCT, '_1567_voluntaryExit_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patientDied</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Died</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_phoneWhyNot_99DCT, '_160034_died_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_phoneWhyNot_99DCT, '_5622_other_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notcontactedphysicaly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**_Reason not contacted (Physical)_**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noLocation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No locator information,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_physicalWhyNot_99DCT, '_165073_noLocation_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incorrect_location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_physicalWhyNot_99DCT, '_165072_wrong_location_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Migrated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_physicalWhyNot_99DCT, '_160415_migrated_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notFoundAtHome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not found at home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_physicalWhyNot_99DCT, '_1706_kp_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_physicalWhyNot_99DCT, '_160034_died_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(../../observation/_1779_physicalWhyNot_99DCT, '_5622_otherInfo_99DCT')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r_followup_contacted_linked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Follow Up Tasks &lt;i class="fa fa-flag"&gt;&lt;/i&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${_159811_outcome_99DCT}=”_1065_contactedAndLinked_99DCT”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h1 green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r_followup_note_positive</t>
+    <t>select_one reasons_physical</t>
+  </si>
+  <si>
+    <t>_1779_physicalWhyNot_99DCT</t>
+  </si>
+  <si>
+    <t>Why was physical tracing not successful?</t>
+  </si>
+  <si>
+    <t>${_159811_outcome_99DCT}=”_1118_notReached_99DCT” and ${_164966_tracingType_99DCT}=”_164965_physical_99DCT”</t>
+  </si>
+  <si>
+    <t>_5622_physicalSpecify_99DCT</t>
+  </si>
+  <si>
+    <t>Other (specify)?</t>
+  </si>
+  <si>
+    <t>${_1779_physicalWhyNot_99DCT}=”_5622_otherInfo_99DCT”</t>
+  </si>
+  <si>
+    <t>linkage_alert</t>
+  </si>
+  <si>
+    <t>&lt;span style="color:red;font-weight:bold"&gt;Please fill UPN in the linkage form once you submit this form&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>${_159811_outcome_99DCT}='_1065_contactedAndLinked_99DCT'</t>
+  </si>
+  <si>
+    <t>_5622_remarks_99DCT</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>group_review</t>
+  </si>
+  <si>
+    <t>Summary page</t>
+  </si>
+  <si>
+    <t>field-list summary</t>
+  </si>
+  <si>
+    <t>n_submit</t>
+  </si>
+  <si>
+    <t>_Be sure you submit to complete this action._</t>
+  </si>
+  <si>
+    <t>n_household_details_title</t>
+  </si>
+  <si>
+    <t>Client details&lt;I class="fa fa-user"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>h1 yellow</t>
+  </si>
+  <si>
+    <t>n_household_details</t>
+  </si>
+  <si>
+    <t>&lt;h4 style="text-align:center;"&gt;${place_name} ${head}&lt;/h4&gt;</t>
+  </si>
+  <si>
+    <t>n_assessment_findings</t>
+  </si>
+  <si>
+    <t>Assessment findings&lt;I class="fa fa-user"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>h1 blue</t>
+  </si>
+  <si>
+    <t>tracking</t>
+  </si>
+  <si>
+    <t>**_Contact type_**</t>
+  </si>
+  <si>
+    <t>physical</t>
+  </si>
+  <si>
+    <t>Physical tracing</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_164966_tracingType_99DCT, '_1650_phone_99DCT')</t>
+  </si>
+  <si>
+    <t>li</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Phone tracing</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_164966_tracingType_99DCT, '_164965_physical_99DCT')</t>
+  </si>
+  <si>
+    <t>n_test_1_results</t>
+  </si>
+  <si>
+    <t>**_Status_**</t>
+  </si>
+  <si>
+    <t>contactedAndLinked</t>
+  </si>
+  <si>
+    <t>Contacted and linked</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_159811_outcome_99DCT, '_1065_contactedAndLinked_99DCT')</t>
+  </si>
+  <si>
+    <t>cintactedNotLinked</t>
+  </si>
+  <si>
+    <t>Contacted not linked</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_159811_outcome_99DCT, '_1066_contactedNotLinked_99DCT')</t>
+  </si>
+  <si>
+    <t>voluntaryExit</t>
+  </si>
+  <si>
+    <t>Not contacted</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_159811_outcome_99DCT, '_1118_notReached_99DCT')</t>
+  </si>
+  <si>
+    <t>n_hts_strategy</t>
+  </si>
+  <si>
+    <t>**_Reason not contacted (Phone)_**</t>
+  </si>
+  <si>
+    <t>locationNotAvailable</t>
+  </si>
+  <si>
+    <t>No locator information</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_phoneWhyNot_99DCT, '_165073_locationMissing_99DCT')</t>
+  </si>
+  <si>
+    <t>wrongLocation</t>
+  </si>
+  <si>
+    <t>Incorrect locator information</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_phoneWhyNot_99DCT, '_165072_incorrect_location_99DCT')</t>
+  </si>
+  <si>
+    <t>callsNotGoingThrough</t>
+  </si>
+  <si>
+    <t>Calls not going through</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_phoneWhyNot_99DCT, '_1567_voluntaryExit_99DCT')</t>
+  </si>
+  <si>
+    <t>patientDied</t>
+  </si>
+  <si>
+    <t>Died</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_phoneWhyNot_99DCT, '_160034_died_99DCT')</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_phoneWhyNot_99DCT, '_5622_other_99DCT')</t>
+  </si>
+  <si>
+    <t>notcontactedphysicaly</t>
+  </si>
+  <si>
+    <t>**_Reason not contacted (Physical)_**</t>
+  </si>
+  <si>
+    <t>noLocation</t>
+  </si>
+  <si>
+    <t>No locator information,</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_physicalWhyNot_99DCT, '_165073_noLocation_99DCT')</t>
+  </si>
+  <si>
+    <t>incorrect_location</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_physicalWhyNot_99DCT, '_165072_wrong_location_99DCT')</t>
+  </si>
+  <si>
+    <t>Migrated</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_physicalWhyNot_99DCT, '_160415_migrated_99DCT')</t>
+  </si>
+  <si>
+    <t>notFoundAtHome</t>
+  </si>
+  <si>
+    <t>Not found at home</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_physicalWhyNot_99DCT, '_1706_kp_99DCT')</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_physicalWhyNot_99DCT, '_160034_died_99DCT')</t>
+  </si>
+  <si>
+    <t>selected(../../observation/_1779_physicalWhyNot_99DCT, '_5622_otherInfo_99DCT')</t>
+  </si>
+  <si>
+    <t>r_followup_contacted_linked</t>
+  </si>
+  <si>
+    <t>Follow Up Tasks &lt;i class="fa fa-flag"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>${_159811_outcome_99DCT}=”_1065_contactedAndLinked_99DCT”</t>
+  </si>
+  <si>
+    <t>h1 green</t>
+  </si>
+  <si>
+    <t>r_followup_note_positive</t>
   </si>
   <si>
     <t xml:space="preserve">Please remember to fill referral and linkage form after saving this form </t>
   </si>
   <si>
-    <t xml:space="preserve">selected(../../observation/_159811_outcome_99DCT, '_1065_contactedAndLinked_99DCT’)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1065_yes_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1066_no_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
+    <t>selected(../../observation/_159811_outcome_99DCT, '_1065_contactedAndLinked_99DCT’)</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>yes_no</t>
+  </si>
+  <si>
+    <t>_1065_yes_99DCT</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>_1066_no_99DCT</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t xml:space="preserve"> tracing_type</t>
   </si>
   <si>
-    <t xml:space="preserve">_1650_phone_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_164965_physical_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact_status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1065_contactedAndLinked_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1066_contactedNotLinked_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contacted but not linked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1118_notReached_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasons_phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_165072_incorrect_location_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrong phone number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1567_voluntaryExit_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_160034_died_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_5622_other_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasons_physical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_165073_noLocation_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_165072_wrong_location_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_160415_migrated_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relocated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_1706_notFoundAtHome_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_5622_otherInfo_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">style</t>
-  </si>
-  <si>
-    <t xml:space="preserve">path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">instance_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTS Client Tracing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hts_client_tracing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data</t>
+    <t>_1650_phone_99DCT</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>_164965_physical_99DCT</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>contact_status</t>
+  </si>
+  <si>
+    <t>_1065_contactedAndLinked_99DCT</t>
+  </si>
+  <si>
+    <t>_1066_contactedNotLinked_99DCT</t>
+  </si>
+  <si>
+    <t>Contacted but not linked</t>
+  </si>
+  <si>
+    <t>_1118_notReached_99DCT</t>
+  </si>
+  <si>
+    <t>reasons_phone</t>
+  </si>
+  <si>
+    <t>_165072_incorrect_location_99DCT</t>
+  </si>
+  <si>
+    <t>Wrong phone number</t>
+  </si>
+  <si>
+    <t>_1567_voluntaryExit_99DCT</t>
+  </si>
+  <si>
+    <t>_160034_died_99DCT</t>
+  </si>
+  <si>
+    <t>_5622_other_99DCT</t>
+  </si>
+  <si>
+    <t>reasons_physical</t>
+  </si>
+  <si>
+    <t>_165073_noLocation_99DCT</t>
+  </si>
+  <si>
+    <t>_165072_wrong_location_99DCT</t>
+  </si>
+  <si>
+    <t>_160415_migrated_99DCT</t>
+  </si>
+  <si>
+    <t>Relocated</t>
+  </si>
+  <si>
+    <t>_1706_notFoundAtHome_99DCT</t>
+  </si>
+  <si>
+    <t>_5622_otherInfo_99DCT</t>
+  </si>
+  <si>
+    <t>form_title</t>
+  </si>
+  <si>
+    <t>form_id</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>HTS Client Tracing</t>
+  </si>
+  <si>
+    <t>hts_client_tracing</t>
+  </si>
+  <si>
+    <t>pages</t>
+  </si>
+  <si>
+    <t>data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="DD\-MM\-YYYY\ HH\-MM\-SS"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -655,22 +668,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -716,21 +714,18 @@
       <sz val="11"/>
       <color rgb="FF4C4C4C"/>
       <name val="Ubuntu"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -767,14 +762,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFD0CECE"/>
       </left>
@@ -790,402 +785,1018 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+  <dxfs count="104">
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1244,45 +1855,352 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF4C4C4C"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AL65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AL72"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E41" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.7295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.015306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.9081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.1377551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="41.6683673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="94.4030612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.9081632653061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.9081632653061"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="17.9081632653061"/>
+    <col min="1" max="1" width="35.73046875"/>
+    <col min="2" max="2" width="43"/>
+    <col min="3" max="3" width="62"/>
+    <col min="4" max="4" width="17.9296875"/>
+    <col min="5" max="5" width="74.86328125"/>
+    <col min="6" max="6" width="21.9296875"/>
+    <col min="7" max="7" width="49.1328125"/>
+    <col min="8" max="8" width="41.6640625"/>
+    <col min="9" max="9" width="94.3984375"/>
+    <col min="10" max="10" width="17.9296875"/>
+    <col min="11" max="11" width="31.86328125"/>
+    <col min="12" max="12" width="17.9296875"/>
+    <col min="13" max="25" width="37.796875"/>
+    <col min="26" max="1025" width="17.9296875"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:38" ht="13.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1335,7 +2253,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:38" ht="13.5">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1372,7 +2290,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:38" ht="13.5">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1407,7 +2325,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:38" ht="13.5">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1440,7 +2358,7 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:38" ht="13.5">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1473,7 +2391,7 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:38" ht="13.5">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1508,7 +2426,7 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:38" ht="13.5">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1541,7 +2459,7 @@
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:38" ht="15.75">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1587,7 +2505,7 @@
       <c r="AK8" s="7"/>
       <c r="AL8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:38" ht="15.75">
       <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
@@ -1633,7 +2551,7 @@
       <c r="AK9" s="7"/>
       <c r="AL9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:38" ht="13.5">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1666,7 +2584,7 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:38" ht="13.5">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1699,7 +2617,7 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:38" ht="13.5">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1728,7 +2646,7 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:38" ht="13.5">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1757,7 +2675,7 @@
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:38" ht="13.5">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1786,7 +2704,7 @@
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:38" ht="13.5">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -1815,7 +2733,7 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:38" ht="13.5">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
@@ -1850,7 +2768,7 @@
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:25" ht="13.5">
       <c r="A17" s="3" t="s">
         <v>38</v>
       </c>
@@ -1885,7 +2803,7 @@
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:25" ht="13.5">
       <c r="A18" s="8" t="s">
         <v>38</v>
       </c>
@@ -1920,7 +2838,7 @@
       <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:25" ht="13.5">
       <c r="A19" s="8" t="s">
         <v>38</v>
       </c>
@@ -1955,7 +2873,7 @@
       <c r="X19" s="8"/>
       <c r="Y19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:25" ht="13.5">
       <c r="A20" s="8" t="s">
         <v>38</v>
       </c>
@@ -1990,7 +2908,7 @@
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:25" ht="13.5">
       <c r="A21" s="8" t="s">
         <v>38</v>
       </c>
@@ -2025,7 +2943,7 @@
       <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
     </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:25" ht="13.5">
       <c r="A22" s="8" t="s">
         <v>38</v>
       </c>
@@ -2060,7 +2978,7 @@
       <c r="X22" s="8"/>
       <c r="Y22" s="8"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:25" ht="13.5">
       <c r="A23" s="8" t="s">
         <v>52</v>
       </c>
@@ -2099,7 +3017,7 @@
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:25" ht="13.5">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2126,7 +3044,7 @@
       <c r="X24" s="8"/>
       <c r="Y24" s="8"/>
     </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:25" ht="13.5">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2153,7 +3071,7 @@
       <c r="X25" s="8"/>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:25" ht="14.25">
       <c r="A26" s="8" t="s">
         <v>13</v>
       </c>
@@ -2188,7 +3106,7 @@
       <c r="X26" s="8"/>
       <c r="Y26" s="8"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:25" ht="13.5">
       <c r="A27" s="8" t="s">
         <v>60</v>
       </c>
@@ -2223,7 +3141,7 @@
       <c r="X27" s="8"/>
       <c r="Y27" s="8"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:25" ht="15.4">
       <c r="A28" s="11" t="s">
         <v>63</v>
       </c>
@@ -2250,7 +3168,7 @@
       <c r="Q28" s="15"/>
       <c r="U28" s="15"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:25" ht="15.4">
       <c r="A29" s="11" t="s">
         <v>63</v>
       </c>
@@ -2277,7 +3195,7 @@
       <c r="Q29" s="15"/>
       <c r="U29" s="15"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:25" ht="13.5">
       <c r="A30" s="8" t="s">
         <v>70</v>
       </c>
@@ -2312,7 +3230,7 @@
       <c r="X30" s="8"/>
       <c r="Y30" s="8"/>
     </row>
-    <row r="31" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:25" ht="27">
       <c r="A31" s="8" t="s">
         <v>73</v>
       </c>
@@ -2349,7 +3267,7 @@
       <c r="X31" s="8"/>
       <c r="Y31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:25" ht="13.5">
       <c r="A32" s="8" t="s">
         <v>77</v>
       </c>
@@ -2386,7 +3304,7 @@
       <c r="X32" s="8"/>
       <c r="Y32" s="8"/>
     </row>
-    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:25" ht="13.5">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2413,7 +3331,7 @@
       <c r="X33" s="8"/>
       <c r="Y33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:25" ht="13.5">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -2440,7 +3358,7 @@
       <c r="X34" s="8"/>
       <c r="Y34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:25" ht="27">
       <c r="A35" s="8" t="s">
         <v>82</v>
       </c>
@@ -2477,7 +3395,7 @@
       <c r="X35" s="8"/>
       <c r="Y35" s="8"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:25" ht="13.5">
       <c r="A36" s="8" t="s">
         <v>77</v>
       </c>
@@ -2514,7 +3432,7 @@
       <c r="X36" s="8"/>
       <c r="Y36" s="8"/>
     </row>
-    <row r="37" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:25" ht="27">
       <c r="A37" s="8" t="s">
         <v>63</v>
       </c>
@@ -2549,7 +3467,7 @@
       <c r="X37" s="8"/>
       <c r="Y37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:25" ht="13.5">
       <c r="A38" s="8" t="s">
         <v>77</v>
       </c>
@@ -2584,7 +3502,7 @@
       <c r="X38" s="8"/>
       <c r="Y38" s="8"/>
     </row>
-    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:25" ht="13.5">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -2611,7 +3529,7 @@
       <c r="X39" s="8"/>
       <c r="Y39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:25" ht="13.5">
       <c r="A40" s="8" t="s">
         <v>37</v>
       </c>
@@ -2640,7 +3558,7 @@
       <c r="X40" s="8"/>
       <c r="Y40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:25" ht="13.5">
       <c r="A41" s="4"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -2667,7 +3585,7 @@
       <c r="X41" s="8"/>
       <c r="Y41" s="8"/>
     </row>
-    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:25" ht="13.5">
       <c r="A43" s="4" t="s">
         <v>13</v>
       </c>
@@ -2702,7 +3620,7 @@
       <c r="X43" s="8"/>
       <c r="Y43" s="8"/>
     </row>
-    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:25" ht="13.5">
       <c r="A44" s="4" t="s">
         <v>63</v>
       </c>
@@ -2735,7 +3653,7 @@
       <c r="X44" s="8"/>
       <c r="Y44" s="8"/>
     </row>
-    <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:25" ht="13.5">
       <c r="A45" s="4" t="s">
         <v>63</v>
       </c>
@@ -2770,7 +3688,7 @@
       <c r="X45" s="8"/>
       <c r="Y45" s="8"/>
     </row>
-    <row r="46" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:25" ht="13.5">
       <c r="A46" s="4" t="s">
         <v>63</v>
       </c>
@@ -2803,7 +3721,7 @@
       <c r="X46" s="8"/>
       <c r="Y46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:25" ht="13.5">
       <c r="A47" s="4" t="s">
         <v>63</v>
       </c>
@@ -2838,7 +3756,7 @@
       <c r="X47" s="8"/>
       <c r="Y47" s="8"/>
     </row>
-    <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:25" ht="13.5">
       <c r="A48" s="4" t="s">
         <v>63</v>
       </c>
@@ -2871,7 +3789,7 @@
       <c r="X48" s="4"/>
       <c r="Y48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:25" ht="13.5">
       <c r="A49" s="4" t="s">
         <v>63</v>
       </c>
@@ -2883,7 +3801,7 @@
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>112</v>
@@ -2908,7 +3826,7 @@
       <c r="X49" s="4"/>
       <c r="Y49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:25" ht="17.45" customHeight="1">
       <c r="A50" s="4" t="s">
         <v>63</v>
       </c>
@@ -2920,7 +3838,7 @@
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>112</v>
@@ -2945,7 +3863,7 @@
       <c r="X50" s="4"/>
       <c r="Y50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:25" ht="17.45" customHeight="1">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="18"/>
@@ -2972,7 +3890,7 @@
       <c r="X51" s="4"/>
       <c r="Y51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:25" ht="13.5">
       <c r="A52" s="8" t="s">
         <v>63</v>
       </c>
@@ -3005,7 +3923,7 @@
       <c r="X52" s="8"/>
       <c r="Y52" s="8"/>
     </row>
-    <row r="53" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:25" ht="27">
       <c r="A53" s="4" t="s">
         <v>63</v>
       </c>
@@ -3042,7 +3960,7 @@
       <c r="X53" s="8"/>
       <c r="Y53" s="8"/>
     </row>
-    <row r="54" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:25" ht="27">
       <c r="A54" s="4" t="s">
         <v>63</v>
       </c>
@@ -3079,7 +3997,7 @@
       <c r="X54" s="8"/>
       <c r="Y54" s="8"/>
     </row>
-    <row r="55" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:25" ht="13.5">
       <c r="A55" s="4" t="s">
         <v>63</v>
       </c>
@@ -3116,7 +4034,7 @@
       <c r="X55" s="8"/>
       <c r="Y55" s="8"/>
     </row>
-    <row r="56" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:25" ht="27">
       <c r="A56" s="8" t="s">
         <v>63</v>
       </c>
@@ -3151,7 +4069,7 @@
       <c r="X56" s="8"/>
       <c r="Y56" s="8"/>
     </row>
-    <row r="57" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:25" ht="27">
       <c r="A57" s="4" t="s">
         <v>63</v>
       </c>
@@ -3188,7 +4106,7 @@
       <c r="X57" s="4"/>
       <c r="Y57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:25" ht="27">
       <c r="A58" s="4" t="s">
         <v>63</v>
       </c>
@@ -3225,7 +4143,7 @@
       <c r="X58" s="4"/>
       <c r="Y58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:25" ht="27">
       <c r="A59" s="4" t="s">
         <v>63</v>
       </c>
@@ -3262,7 +4180,7 @@
       <c r="X59" s="4"/>
       <c r="Y59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:25" ht="13.5">
       <c r="A60" s="4" t="s">
         <v>63</v>
       </c>
@@ -3299,7 +4217,7 @@
       <c r="X60" s="4"/>
       <c r="Y60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:25" ht="13.5">
       <c r="A61" s="4" t="s">
         <v>63</v>
       </c>
@@ -3336,7 +4254,7 @@
       <c r="X61" s="4"/>
       <c r="Y61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:25" ht="13.5">
       <c r="A62" s="4"/>
       <c r="B62" s="18"/>
       <c r="C62" s="19"/>
@@ -3363,7 +4281,7 @@
       <c r="X62" s="4"/>
       <c r="Y62" s="4"/>
     </row>
-    <row r="63" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:25" ht="27">
       <c r="A63" s="8" t="s">
         <v>63</v>
       </c>
@@ -3398,7 +4316,7 @@
       <c r="X63" s="8"/>
       <c r="Y63" s="8"/>
     </row>
-    <row r="64" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:25" ht="27">
       <c r="A64" s="4" t="s">
         <v>63</v>
       </c>
@@ -3435,7 +4353,7 @@
       <c r="X64" s="4"/>
       <c r="Y64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:25" ht="27">
       <c r="A65" s="4" t="s">
         <v>63</v>
       </c>
@@ -3472,7 +4390,7 @@
       <c r="X65" s="4"/>
       <c r="Y65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:25" ht="27">
       <c r="A66" s="4" t="s">
         <v>63</v>
       </c>
@@ -3509,7 +4427,7 @@
       <c r="X66" s="4"/>
       <c r="Y66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:25" ht="13.5">
       <c r="A67" s="4" t="s">
         <v>63</v>
       </c>
@@ -3546,7 +4464,7 @@
       <c r="X67" s="4"/>
       <c r="Y67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:25" ht="13.5">
       <c r="A68" s="4" t="s">
         <v>63</v>
       </c>
@@ -3583,7 +4501,7 @@
       <c r="X68" s="4"/>
       <c r="Y68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:25" ht="27">
       <c r="A69" s="4" t="s">
         <v>63</v>
       </c>
@@ -3618,7 +4536,7 @@
       <c r="X69" s="4"/>
       <c r="Y69" s="4"/>
     </row>
-    <row r="70" s="12" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:25" s="12" customFormat="1" ht="15.75" customHeight="1">
       <c r="A70" s="20" t="s">
         <v>63</v>
       </c>
@@ -3655,7 +4573,7 @@
       <c r="X70" s="20"/>
       <c r="Y70" s="20"/>
     </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:25" ht="15.75" customHeight="1">
       <c r="A71" s="23" t="s">
         <v>63</v>
       </c>
@@ -3690,7 +4608,7 @@
       <c r="X71" s="23"/>
       <c r="Y71" s="23"/>
     </row>
-    <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:25" ht="13.5">
       <c r="A72" s="4" t="s">
         <v>37</v>
       </c>
@@ -3719,552 +4637,535 @@
       <c r="X72" s="8"/>
       <c r="Y72" s="8"/>
     </row>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" priority="2" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="103" priority="2" operator="notEqual">
       <formula>"name"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="notContainsText" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="0"/>
+    <cfRule type="notContainsText" dxfId="102" priority="3" operator="notContains" text="label"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" priority="4" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="101" priority="4" operator="notEqual">
       <formula>"required"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" priority="5" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="100" priority="5" operator="notEqual">
       <formula>"relevant"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" priority="6" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="99" priority="6" operator="notEqual">
       <formula>"appearance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="7" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="98" priority="7" operator="notEqual">
       <formula>"constraint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="notContainsText" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="0"/>
+    <cfRule type="notContainsText" dxfId="97" priority="8" operator="notContains" text="constraint_message"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" priority="9" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="96" priority="9" operator="notEqual">
       <formula>"calculation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" priority="10" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="95" priority="10" operator="notEqual">
       <formula>"choice_filter"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="notContainsText" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="0"/>
+    <cfRule type="notContainsText" dxfId="94" priority="11" operator="notContains" text="hint"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="93" priority="12" operator="notEqual">
       <formula>"default"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Y1">
-    <cfRule type="cellIs" priority="13" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="92" priority="13" operator="notEqual">
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="91" priority="14" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="90" priority="15" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:I34">
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="89" priority="16">
       <formula>AND($I32 = "", $A32 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C34">
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="88" priority="17">
       <formula>AND(AND(NOT($A32 = "end group"), NOT($A32 = "end repeat"), NOT($A32 = "")), $C32 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:B34">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="87" priority="18">
       <formula>AND(AND(NOT($A32 = "end group"), NOT($A32 = "end repeat"), NOT($A32 = "")), $B32 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:A34">
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="86" priority="19" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H34">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="85" priority="20">
       <formula>AND(NOT($G32 = ""), $H32 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+    <cfRule type="containsText" dxfId="84" priority="21" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="83" priority="22">
       <formula>AND($A31="begin group", NOT($B31 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="82" priority="23">
       <formula>AND($A31="end group", $B31 = "", $C31 = "", $D31 = "", $E31 = "", $F31 = "", $G31 = "", $H31 = "", $I31 = "", $J31 = "", $K31 = "", $L31 = "", $M31 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="81" priority="24" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="80" priority="25">
       <formula>AND($A31="begin repeat", NOT($B31 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="79" priority="26">
       <formula>AND($A31="end repeat", $B31 = "", $C31 = "", $D31 = "", $E31 = "", $F31 = "", $G31 = "", $H31 = "", $I31 = "", $J31 = "", $K31 = "", $L31 = "", $M31 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="78" priority="27">
       <formula>AND($I38 = "", $A38 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="expression" dxfId="77" priority="28">
       <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $C38 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" dxfId="76" priority="29">
       <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $B38 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" dxfId="75" priority="30" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" dxfId="74" priority="31">
       <formula>AND(NOT($G38 = ""), $H38 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:Y25">
-    <cfRule type="containsText" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="4"/>
+    <cfRule type="containsText" dxfId="73" priority="32" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:Y25">
-    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="72" priority="33" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="71" priority="34" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="containsText" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="6"/>
+    <cfRule type="containsText" dxfId="70" priority="35" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" dxfId="69" priority="36">
       <formula>AND($A72="begin group", NOT($B72 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="68" priority="37">
       <formula>AND($A72="end group", $B72 = "", $C72 = "", $D72 = "", $E72 = "", $F72 = "", $G72 = "", $H72 = "", $I72 = "", $J72 = "", $K72 = "", $L72 = "", $M72 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" dxfId="67" priority="38" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="cellIs" priority="39" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" dxfId="66" priority="39" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="65" priority="40">
       <formula>AND($A72="begin repeat", NOT($B72 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="64" priority="41">
       <formula>AND($A72="end repeat", $B72 = "", $C72 = "", $D72 = "", $E72 = "", $F72 = "", $G72 = "", $H72 = "", $I72 = "", $J72 = "", $K72 = "", $L72 = "", $M72 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="63" priority="42">
       <formula>AND($I35 = "", $A35 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="62" priority="43">
       <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $C35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="61" priority="44">
       <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $B35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="cellIs" priority="45" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" dxfId="60" priority="45" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="59" priority="46">
       <formula>AND(NOT($G35 = ""), $H35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="expression" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="58" priority="47">
       <formula>AND($I36 = "", $A36 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" priority="48" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="57" priority="48">
       <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $C36 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" priority="49" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="56" priority="49">
       <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $B36 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" dxfId="55" priority="50" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="54" priority="51">
       <formula>AND(NOT($G36 = ""), $H36 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="containsText" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" dxfId="52" priority="53">
       <formula>AND($A36="begin group", NOT($B36 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="54" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="expression" dxfId="51" priority="54">
       <formula>AND($A36="end group", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" priority="55" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" dxfId="50" priority="55" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="56" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" dxfId="49" priority="56">
       <formula>AND($A36="begin repeat", NOT($B36 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" dxfId="48" priority="57">
       <formula>AND($A36="end repeat", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="containsText" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="12"/>
+    <cfRule type="containsText" dxfId="47" priority="58" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" dxfId="46" priority="59">
       <formula>AND($A35="begin group", NOT($B35 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" dxfId="45" priority="60">
       <formula>AND($A35="end group", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $G35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" priority="61" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" dxfId="44" priority="61" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" dxfId="43" priority="62">
       <formula>AND($A35="begin repeat", NOT($B35 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" dxfId="42" priority="63">
       <formula>AND($A35="end repeat", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $G35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="containsText" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="13"/>
+    <cfRule type="containsText" dxfId="41" priority="64" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" dxfId="40" priority="65">
       <formula>AND($A52="begin group", NOT($B52 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" dxfId="39" priority="66">
       <formula>AND($A52="end group", $B52 = "", $C52 = "", $D52 = "", $E52 = "", $F52 = "", $G52 = "", $H52 = "", $I52 = "", $J52 = "", $K52 = "", $L52 = "", $M52 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="cellIs" dxfId="38" priority="67" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" dxfId="37" priority="68">
       <formula>AND($A52="begin repeat", NOT($B52 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" dxfId="36" priority="69">
       <formula>AND($A52="end repeat", $B52 = "", $C52 = "", $D52 = "", $E52 = "", $F52 = "", $G52 = "", $H52 = "", $I52 = "", $J52 = "", $K52 = "", $L52 = "", $M52 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" priority="70" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="cellIs" dxfId="35" priority="70" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="containsText" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="14"/>
+    <cfRule type="containsText" dxfId="34" priority="71" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" dxfId="33" priority="72">
       <formula>AND($A54="begin group", NOT($B54 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" dxfId="32" priority="73">
       <formula>AND($A54="end group", $B54 = "", $C54 = "", $D54 = "", $E54 = "", $F54 = "", $G54 = "", $H54 = "", $I54 = "", $J54 = "", $K54 = "", $L54 = "", $M54 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="cellIs" priority="74" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="cellIs" dxfId="31" priority="74" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54">
-    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" dxfId="30" priority="75">
       <formula>AND($I54 = "", $A54 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" dxfId="29" priority="76">
       <formula>AND(AND(NOT($A54 = "end group"), NOT($A54 = "end repeat"), NOT($A54 = "")), $C54 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" dxfId="28" priority="77">
       <formula>AND(AND(NOT($A54 = "end group"), NOT($A54 = "end repeat"), NOT($A54 = "")), $B54 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54">
-    <cfRule type="cellIs" priority="78" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" dxfId="27" priority="78" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" dxfId="26" priority="79">
       <formula>AND(NOT($G54 = ""), $H54 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" dxfId="25" priority="80">
       <formula>AND($A54="begin repeat", NOT($B54 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:Y54">
-    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" dxfId="24" priority="81">
       <formula>AND($A54="end repeat", $B54 = "", $C54 = "", $D54 = "", $E54 = "", $F54 = "", $G54 = "", $H54 = "", $I54 = "", $J54 = "", $K54 = "", $L54 = "", $M54 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="containsText" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="17"/>
+    <cfRule type="containsText" dxfId="23" priority="82" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="expression" dxfId="22" priority="83">
       <formula>AND($A55="begin group", NOT($B55 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="expression" dxfId="21" priority="84">
       <formula>AND($A55="end group", $B55 = "", $C55 = "", $D55 = "", $E55 = "", $F55 = "", $G55 = "", $H55 = "", $I55 = "", $J55 = "", $K55 = "", $L55 = "", $M55 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="cellIs" dxfId="20" priority="85" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55">
-    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="expression" dxfId="19" priority="86">
       <formula>AND($I55 = "", $A55 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
-    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="expression" dxfId="18" priority="87">
       <formula>AND(AND(NOT($A55 = "end group"), NOT($A55 = "end repeat"), NOT($A55 = "")), $C55 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+    <cfRule type="expression" dxfId="17" priority="88">
       <formula>AND(AND(NOT($A55 = "end group"), NOT($A55 = "end repeat"), NOT($A55 = "")), $B55 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55">
-    <cfRule type="cellIs" priority="89" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="cellIs" dxfId="16" priority="89" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+    <cfRule type="expression" dxfId="15" priority="90">
       <formula>AND(NOT($G55 = ""), $H55 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+    <cfRule type="expression" dxfId="14" priority="91">
       <formula>AND($A55="begin repeat", NOT($B55 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+    <cfRule type="expression" dxfId="13" priority="92">
       <formula>AND($A55="end repeat", $B55 = "", $C55 = "", $D55 = "", $E55 = "", $F55 = "", $G55 = "", $H55 = "", $I55 = "", $J55 = "", $K55 = "", $L55 = "", $M55 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+    <cfRule type="expression" dxfId="12" priority="93">
       <formula>AND(A1 = "type", COUNTIF($A$1:$A$984, "begin group") = COUNTIF($A$1:$A$984, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+    <cfRule type="expression" dxfId="11" priority="94">
       <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$975, "begin group") = COUNTIF($A$1:$A$984, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="10" priority="95">
       <formula>AND($I37 = "", $A37 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" priority="96" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="9" priority="96">
       <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $C37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="8" priority="97">
       <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $B37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="cellIs" priority="98" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" dxfId="7" priority="98" operator="equal">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="6" priority="99">
       <formula>AND(NOT($G37 = ""), $H37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="containsText" priority="100" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+    <cfRule type="containsText" dxfId="5" priority="100" operator="containsText" text="calculate"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="4" priority="101">
       <formula>AND($A37="begin group", NOT($B37 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="3" priority="102">
       <formula>AND($A37="end group", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" dxfId="2" priority="103" operator="equal">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="1" priority="104">
       <formula>AND($A37="begin repeat", NOT($B37 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" dxfId="0" priority="105">
       <formula>AND($A37="end repeat", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D7 D10:D27 D30:D41 D43:D69 D72" type="list">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D7 D10:D27 D30:D41 D43:D69 D72" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="db:universal_client"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F1048538"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.9642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.9081632653061"/>
+    <col min="1" max="1" width="32.59765625"/>
+    <col min="2" max="2" width="39.59765625"/>
+    <col min="3" max="3" width="56.9296875"/>
+    <col min="4" max="1025" width="17.9296875"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="13.9">
       <c r="A1" s="25" t="s">
         <v>165</v>
       </c>
@@ -4278,7 +5179,7 @@
       <c r="E1" s="26"/>
       <c r="F1" s="26"/>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="13.5">
       <c r="A2" s="18" t="s">
         <v>166</v>
       </c>
@@ -4289,7 +5190,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" ht="13.5">
       <c r="A3" s="18" t="s">
         <v>166</v>
       </c>
@@ -4300,12 +5201,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" ht="13.5">
       <c r="A4" s="18"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6">
       <c r="A5" s="19" t="s">
         <v>171</v>
       </c>
@@ -4316,7 +5217,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6">
       <c r="A6" s="19" t="s">
         <v>171</v>
       </c>
@@ -4327,12 +5228,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6">
       <c r="A8" s="19" t="s">
         <v>176</v>
       </c>
@@ -4343,7 +5244,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6">
       <c r="A9" s="19" t="s">
         <v>176</v>
       </c>
@@ -4354,7 +5255,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6">
       <c r="A10" s="19" t="s">
         <v>176</v>
       </c>
@@ -4365,13 +5266,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>181</v>
       </c>
       <c r="B12" s="19" t="s">
@@ -4381,8 +5282,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
         <v>181</v>
       </c>
       <c r="B13" s="19" t="s">
@@ -4392,8 +5293,8 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
         <v>181</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -4403,8 +5304,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
         <v>181</v>
       </c>
       <c r="B15" s="19" t="s">
@@ -4414,12 +5315,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6">
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>187</v>
       </c>
       <c r="B17" s="19" t="s">
@@ -4429,8 +5330,8 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>187</v>
       </c>
       <c r="B18" s="19" t="s">
@@ -4440,8 +5341,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>187</v>
       </c>
       <c r="B19" s="19" t="s">
@@ -4451,8 +5352,8 @@
         <v>191</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>187</v>
       </c>
       <c r="B20" s="19" t="s">
@@ -4462,8 +5363,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
         <v>187</v>
       </c>
       <c r="B21" s="19" t="s">
@@ -4473,8 +5374,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>187</v>
       </c>
       <c r="B22" s="19" t="s">
@@ -4484,41 +5385,31 @@
         <v>142</v>
       </c>
     </row>
-    <row r="1048538" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.9081632653061"/>
+    <col min="1" max="1" width="34.73046875"/>
+    <col min="2" max="2" width="31.33203125"/>
+    <col min="3" max="3" width="29.1328125"/>
+    <col min="4" max="1025" width="17.9296875"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="13.9">
       <c r="A1" s="25" t="s">
         <v>194</v>
       </c>
@@ -4538,16 +5429,16 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="13.5">
       <c r="A2" s="18" t="s">
         <v>200</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="C2" s="28" t="n">
-        <f aca="true">NOW()</f>
-        <v>44347.4972521824</v>
+      <c r="C2" s="28">
+        <f ca="1">NOW()</f>
+        <v>44356.90779409722</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>202</v>
@@ -4557,14 +5448,9 @@
       </c>
       <c r="F2" s="18"/>
     </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>